<commit_message>
Add estado civil  e genero
</commit_message>
<xml_diff>
--- a/Funcionalidade.xlsx
+++ b/Funcionalidade.xlsx
@@ -14,8 +14,8 @@
     <sheet name="funcionalidade (2)" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">funcionalidade!$A$4:$H$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">funcionalidade!$A$4:$H$74</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">funcionalidade!$A$4:$H$74</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">funcionalidade!$A$4:$H$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">data</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-01-04-22-04</t>
+    <t xml:space="preserve">2026-01-05-11-40</t>
   </si>
   <si>
     <t xml:space="preserve">pk_funcionalidade</t>
@@ -3333,7 +3333,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:H4"/>
+  <autoFilter ref="A4:H74"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Tudo funcionado (toda parta da segurança, e fazer denúncia apenas no menu água)
</commit_message>
<xml_diff>
--- a/Funcionalidade.xlsx
+++ b/Funcionalidade.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="funcionalidade" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,8 +14,8 @@
     <sheet name="funcionalidade (2)" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">funcionalidade!$A$4:$H$74</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">funcionalidade!$A$4:$H$4</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">funcionalidade!$A$4:$H$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">funcionalidade!$A$4:$H$74</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">data</t>
   </si>
   <si>
-    <t xml:space="preserve">2026-01-05-11-40</t>
+    <t xml:space="preserve">2026-01-10-12-19</t>
   </si>
   <si>
     <t xml:space="preserve">pk_funcionalidade</t>
@@ -1577,7 +1577,7 @@
   </sheetPr>
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3333,7 +3333,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:H74"/>
+  <autoFilter ref="A4:H4"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3352,7 +3352,7 @@
   </sheetPr>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3834,7 +3834,7 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4888,7 +4888,7 @@
   </sheetPr>
   <dimension ref="A1:AC1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C131" activeCellId="0" sqref="C131"/>

</xml_diff>